<commit_message>
selenium ide code added for landing page
</commit_message>
<xml_diff>
--- a/Akash/Test Template Document Corp Akash Dhole.xlsx
+++ b/Akash/Test Template Document Corp Akash Dhole.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\NCS2\Akash\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -190,9 +190,6 @@
     <t>Test Executed Date</t>
   </si>
   <si>
-    <t>https://demo.openemr.io/b/openemr</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actual Result </t>
   </si>
   <si>
@@ -295,18 +292,6 @@
   </si>
   <si>
     <t>User should be navigated to the dashboard screen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Title should be "OrangeHRM" 
-2. OrangeHRM Logo should be present
-3. Textbox for enterning Username and Password
-4. Textbox should contain Username and Password placeholder.
-5. Login button should be present
-6. Link for "Forgot Your Passsword?" should be present
-7. OrangeHRM verion should be present as "OrangeHRM 4.2"
-8. Copyright detail should be present as "© 2005 - 2022 OrangeHRM, Inc. All rights reserved."
-9. Icon for Linkedin,Facebook,Twitter,Youtube should be pesent. 
-</t>
   </si>
   <si>
     <t>TC_OH_3</t>
@@ -767,6 +752,54 @@
     <t xml:space="preserve">1. Navigate to the Forget password page.
 2. Type Valid Username 
 3. Click on "Reset Password" button </t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. Title should be "OrangeHRM" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2. OrangeHRM Logo should be present
+3. Textbox for enterning Username and Password
+4. Textbox should contain Username and Password placeholder.
+5. Login button should be present
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6. Link for "Forgot Your Passsword?" should be present</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+7. OrangeHRM verion should be present as "OrangeHRM 4.2"
+8. Copyright detail should be present as "© 2005 - 2022 OrangeHRM, Inc. All rights reserved."
+9. Icon for Linkedin,Facebook,Twitter,Youtube should be pesent. 
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1189,6 +1222,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1212,15 +1254,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1263,7 +1296,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1337,7 +1370,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1700,11 +1733,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" s="4" customFormat="1" ht="22.5">
-      <c r="B4" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="B4" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="2:4" s="5" customFormat="1" ht="15">
       <c r="C5" s="6"/>
@@ -1713,28 +1746,28 @@
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="42"/>
+      <c r="C7" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="2:4" ht="17.25" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="42"/>
+      <c r="C8" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="45"/>
     </row>
     <row r="9" spans="2:4" ht="31.5" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="44"/>
+      <c r="C9" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="47"/>
     </row>
     <row r="10" spans="2:4" ht="17.25" customHeight="1">
       <c r="B10" s="9"/>
@@ -1754,10 +1787,10 @@
     </row>
     <row r="13" spans="2:4" ht="13.5">
       <c r="B13" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="11">
         <v>44607</v>
@@ -1776,10 +1809,10 @@
     </row>
     <row r="15" spans="2:4" ht="13.5">
       <c r="B15" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="11"/>
     </row>
@@ -1796,7 +1829,7 @@
     </row>
     <row r="17" spans="2:4" ht="13.5">
       <c r="B17" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="11"/>
@@ -1826,7 +1859,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
@@ -1839,15 +1872,15 @@
   <sheetData>
     <row r="2" spans="1:4" ht="17.649999999999999">
       <c r="C2" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>31</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="13.15">
@@ -1856,7 +1889,7 @@
     </row>
     <row r="6" spans="1:4" ht="15">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -1870,13 +1903,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="15">
         <v>1</v>
@@ -1884,85 +1917,85 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>117</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" s="15"/>
     </row>
@@ -2005,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -2046,13 +2079,13 @@
         <v>19</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="J1" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>29</v>
@@ -2068,25 +2101,25 @@
       <c r="A2" s="33"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:13" s="21" customFormat="1" ht="140.25">
+    <row r="3" spans="1:13" s="21" customFormat="1" ht="141">
       <c r="A3" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="E3" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>58</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="35" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="K3" s="39">
         <v>44607</v>
@@ -2094,25 +2127,25 @@
     </row>
     <row r="4" spans="1:13" s="21" customFormat="1" ht="51">
       <c r="A4" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="D4" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="35" t="s">
+      <c r="F4" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="G4" s="35" t="s">
         <v>63</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="38">
         <v>44607</v>
@@ -2120,608 +2153,608 @@
     </row>
     <row r="5" spans="1:13" s="21" customFormat="1" ht="89.25">
       <c r="A5" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>68</v>
-      </c>
       <c r="G5" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="21" customFormat="1" ht="51">
       <c r="A6" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>71</v>
-      </c>
       <c r="G6" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="21" customFormat="1" ht="51">
       <c r="A7" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A8" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="F8" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>82</v>
-      </c>
       <c r="G8" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A9" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A10" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="35" t="s">
         <v>98</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>100</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A11" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A12" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="35" t="s">
-        <v>96</v>
-      </c>
       <c r="D12" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="21" customFormat="1" ht="38.25">
       <c r="A13" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>97</v>
-      </c>
       <c r="D13" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="21" customFormat="1" ht="191.25">
       <c r="A14" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="D14" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="21" customFormat="1" ht="144" customHeight="1">
       <c r="A15" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>121</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="21" customFormat="1" ht="114.75">
       <c r="A16" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="35" t="s">
+      <c r="G16" s="35" t="s">
         <v>125</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="21" customFormat="1" ht="89.25">
       <c r="A17" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A18" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C18" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="35" t="s">
         <v>145</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A19" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A20" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A21" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A22" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A23" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A24" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="35" t="s">
         <v>162</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A25" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="21" customFormat="1" ht="76.5">
       <c r="A26" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A27" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A28" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="21" customFormat="1" ht="51">
       <c r="A29" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="21" customFormat="1" ht="140.25">
+      <c r="A30" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G29" s="35" t="s">
+      <c r="F30" s="42"/>
+      <c r="G30" s="41" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="21" customFormat="1" ht="140.25">
-      <c r="A30" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="49" t="s">
-        <v>188</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="D30" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="49" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="21" customFormat="1" ht="63.75">
       <c r="A31" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F31" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="35" t="s">
         <v>180</v>
-      </c>
-      <c r="G31" s="35" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="21" customFormat="1"/>
@@ -3140,14 +3173,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.399999999999999" thickTop="1" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" thickTop="1" thickBot="1">
       <c r="A2" s="22"/>
@@ -3261,10 +3294,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3273,18 +3302,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -3454,7 +3476,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -3462,26 +3503,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3498,4 +3520,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>